<commit_message>
Almost simple delta hedge
</commit_message>
<xml_diff>
--- a/source/JoshiProject1.xlsx
+++ b/source/JoshiProject1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="84">
   <si>
     <t>Spot</t>
   </si>
@@ -258,6 +258,18 @@
   <si>
     <t>Note the lower price for the asian due to averaging reducing volatility of stock</t>
   </si>
+  <si>
+    <t xml:space="preserve">spot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">r </t>
+  </si>
+  <si>
+    <t xml:space="preserve">d </t>
+  </si>
+  <si>
+    <t xml:space="preserve">vol </t>
+  </si>
 </sst>
 </file>
 
@@ -1707,11 +1719,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="54880128"/>
-        <c:axId val="54886784"/>
+        <c:axId val="51616384"/>
+        <c:axId val="51623040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="54880128"/>
+        <c:axId val="51616384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1736,12 +1748,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54886784"/>
+        <c:crossAx val="51623040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="54886784"/>
+        <c:axId val="51623040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1767,7 +1779,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54880128"/>
+        <c:crossAx val="51616384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1779,7 +1791,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000777" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000777" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001044" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001044" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2153,11 +2165,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="59010432"/>
-        <c:axId val="59033088"/>
+        <c:axId val="55964032"/>
+        <c:axId val="55965952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59010432"/>
+        <c:axId val="55964032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2182,12 +2194,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59033088"/>
+        <c:crossAx val="55965952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59033088"/>
+        <c:axId val="55965952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2213,7 +2225,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59010432"/>
+        <c:crossAx val="55964032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2222,7 +2234,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000566" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000566" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2263,7 +2275,7 @@
           <c:x val="0.13449220121370181"/>
           <c:y val="0.1299886993292505"/>
           <c:w val="0.82601200327666047"/>
-          <c:h val="0.67880686789151579"/>
+          <c:h val="0.67880686789151878"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2612,11 +2624,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="59046144"/>
-        <c:axId val="58814848"/>
+        <c:axId val="56125696"/>
+        <c:axId val="56136064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59046144"/>
+        <c:axId val="56125696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2645,12 +2657,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58814848"/>
+        <c:crossAx val="56136064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58814848"/>
+        <c:axId val="56136064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2676,7 +2688,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59046144"/>
+        <c:crossAx val="56125696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2685,7 +2697,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000555" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000555" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3065,11 +3077,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="58818560"/>
-        <c:axId val="58844288"/>
+        <c:axId val="56295424"/>
+        <c:axId val="56297344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58818560"/>
+        <c:axId val="56295424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3099,12 +3111,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58844288"/>
+        <c:crossAx val="56297344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58844288"/>
+        <c:axId val="56297344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3114,7 +3126,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58818560"/>
+        <c:crossAx val="56295424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3123,7 +3135,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3503,11 +3515,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="58848384"/>
-        <c:axId val="59054720"/>
+        <c:axId val="56313344"/>
+        <c:axId val="56315264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58848384"/>
+        <c:axId val="56313344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3536,12 +3548,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59054720"/>
+        <c:crossAx val="56315264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59054720"/>
+        <c:axId val="56315264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3551,7 +3563,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58848384"/>
+        <c:crossAx val="56313344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3560,7 +3572,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3941,11 +3953,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="59062912"/>
-        <c:axId val="65212800"/>
+        <c:axId val="56359936"/>
+        <c:axId val="56243328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59062912"/>
+        <c:axId val="56359936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3956,12 +3968,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65212800"/>
+        <c:crossAx val="56243328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65212800"/>
+        <c:axId val="56243328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3973,7 +3985,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59062912"/>
+        <c:crossAx val="56359936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3982,7 +3994,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4361,11 +4373,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="65225088"/>
-        <c:axId val="65230720"/>
+        <c:axId val="56255232"/>
+        <c:axId val="56257152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65225088"/>
+        <c:axId val="56255232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4395,12 +4407,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65230720"/>
+        <c:crossAx val="56257152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="65230720"/>
+        <c:axId val="56257152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4410,7 +4422,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65225088"/>
+        <c:crossAx val="56255232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4419,7 +4431,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4435,7 +4447,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.26891632006966854"/>
+          <c:x val="0.26891632006967053"/>
           <c:y val="2.8275009877756652E-2"/>
           <c:w val="0.6738373047041657"/>
           <c:h val="0.8971166436276885"/>
@@ -5763,23 +5775,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53479296"/>
-        <c:axId val="53480832"/>
+        <c:axId val="41499264"/>
+        <c:axId val="41513344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53479296"/>
+        <c:axId val="41499264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53480832"/>
+        <c:crossAx val="41513344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53480832"/>
+        <c:axId val="41513344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5787,7 +5799,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53479296"/>
+        <c:crossAx val="41499264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5799,7 +5811,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000777" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000777" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001044" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001044" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5837,8 +5849,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10951222115528925"/>
-          <c:y val="6.4986002424439436E-3"/>
+          <c:x val="0.10951222115529009"/>
+          <c:y val="6.4986002424439783E-3"/>
         </c:manualLayout>
       </c:layout>
     </c:title>
@@ -5850,7 +5862,7 @@
           <c:yMode val="edge"/>
           <c:x val="8.4488407699037621E-2"/>
           <c:y val="0.19461706996942271"/>
-          <c:w val="0.85871446655283545"/>
+          <c:w val="0.85871446655283845"/>
           <c:h val="0.63890604507981763"/>
         </c:manualLayout>
       </c:layout>
@@ -6191,23 +6203,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53512832"/>
-        <c:axId val="53531008"/>
+        <c:axId val="41528704"/>
+        <c:axId val="52167808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53512832"/>
+        <c:axId val="41528704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53531008"/>
+        <c:crossAx val="52167808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="53531008"/>
+        <c:axId val="52167808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6215,7 +6227,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53512832"/>
+        <c:crossAx val="41528704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6224,7 +6236,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000755" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000755" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001021" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001021" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6578,23 +6590,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="53542272"/>
-        <c:axId val="57554048"/>
+        <c:axId val="52203904"/>
+        <c:axId val="52205440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="53542272"/>
+        <c:axId val="52203904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57554048"/>
+        <c:crossAx val="52205440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57554048"/>
+        <c:axId val="52205440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6602,7 +6614,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53542272"/>
+        <c:crossAx val="52203904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6614,7 +6626,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000755" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000755" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001021" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001021" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6915,11 +6927,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="57574144"/>
-        <c:axId val="57576064"/>
+        <c:axId val="52213248"/>
+        <c:axId val="52215168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57574144"/>
+        <c:axId val="52213248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6948,12 +6960,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57576064"/>
+        <c:crossAx val="52215168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57576064"/>
+        <c:axId val="52215168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6983,7 +6995,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57574144"/>
+        <c:crossAx val="52213248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6992,7 +7004,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000755" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000755" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001021" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001021" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7372,11 +7384,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="58674176"/>
-        <c:axId val="58680448"/>
+        <c:axId val="54759424"/>
+        <c:axId val="54761344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58674176"/>
+        <c:axId val="54759424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7401,12 +7413,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58680448"/>
+        <c:crossAx val="54761344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58680448"/>
+        <c:axId val="54761344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7436,7 +7448,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58674176"/>
+        <c:crossAx val="54759424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7445,7 +7457,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000677" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000677" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7735,23 +7747,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="58705408"/>
-        <c:axId val="58706944"/>
+        <c:axId val="54774016"/>
+        <c:axId val="54788096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58705408"/>
+        <c:axId val="54774016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58706944"/>
+        <c:crossAx val="54788096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58706944"/>
+        <c:axId val="54788096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7759,7 +7771,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58705408"/>
+        <c:crossAx val="54774016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7771,7 +7783,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000677" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000677" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8335,23 +8347,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="58741888"/>
-        <c:axId val="58743424"/>
+        <c:axId val="54818688"/>
+        <c:axId val="54820224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58741888"/>
+        <c:axId val="54818688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58743424"/>
+        <c:crossAx val="54820224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58743424"/>
+        <c:axId val="54820224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8359,7 +8371,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58741888"/>
+        <c:crossAx val="54818688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8371,7 +8383,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.73931933508311465"/>
-          <c:y val="0.41636293314803657"/>
+          <c:y val="0.41636293314803835"/>
           <c:w val="0.2285784064345967"/>
           <c:h val="0.16727413370393193"/>
         </c:manualLayout>
@@ -8381,7 +8393,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000677" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000677" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8772,23 +8784,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="58993280"/>
-        <c:axId val="59003264"/>
+        <c:axId val="55917952"/>
+        <c:axId val="55936128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58993280"/>
+        <c:axId val="55917952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59003264"/>
+        <c:crossAx val="55936128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59003264"/>
+        <c:axId val="55936128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8796,7 +8808,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58993280"/>
+        <c:crossAx val="55917952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8805,7 +8817,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000566" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000566" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -27879,9 +27891,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:Q256"/>
+  <dimension ref="A2:Q259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
       <selection activeCell="J257" sqref="J257"/>
     </sheetView>
   </sheetViews>
@@ -37687,7 +37699,7 @@
     </row>
     <row r="255" spans="2:13">
       <c r="B255">
-        <f t="shared" ref="B255:B256" si="32">$B$7</f>
+        <f t="shared" ref="B255" si="32">$B$7</f>
         <v>100</v>
       </c>
       <c r="C255">
@@ -37695,7 +37707,7 @@
         <v>0.05</v>
       </c>
       <c r="D255">
-        <f t="shared" ref="D255:D256" si="34">$D$7</f>
+        <f t="shared" ref="D255" si="34">$D$7</f>
         <v>0</v>
       </c>
       <c r="E255">
@@ -37723,16 +37735,14 @@
     </row>
     <row r="256" spans="2:13">
       <c r="B256">
-        <f t="shared" si="32"/>
-        <v>100</v>
+        <v>100.1</v>
       </c>
       <c r="C256">
         <f t="shared" si="33"/>
         <v>0.05</v>
       </c>
       <c r="D256">
-        <f t="shared" si="34"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E256">
         <v>0.15</v>
@@ -37741,17 +37751,53 @@
         <v>1</v>
       </c>
       <c r="G256">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H256">
-        <v>100000</v>
+        <v>10</v>
       </c>
       <c r="I256">
         <v>100</v>
       </c>
       <c r="J256">
         <f>MCDeltaHedge(B256:I256)</f>
-        <v>4.998617445581905</v>
+        <v>1.795162971485383</v>
+      </c>
+      <c r="K256" t="e">
+        <f ca="1">BSDeltaWithParams(B256:I256)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="257" spans="2:10">
+      <c r="B257" t="s">
+        <v>80</v>
+      </c>
+      <c r="C257" t="s">
+        <v>81</v>
+      </c>
+      <c r="D257" t="s">
+        <v>82</v>
+      </c>
+      <c r="E257" t="s">
+        <v>83</v>
+      </c>
+      <c r="F257" t="s">
+        <v>31</v>
+      </c>
+      <c r="G257" t="s">
+        <v>76</v>
+      </c>
+      <c r="H257" t="s">
+        <v>78</v>
+      </c>
+      <c r="I257" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="2:10">
+      <c r="J259" t="e">
+        <f>BS</f>
+        <v>#NAME?</v>
       </c>
     </row>
   </sheetData>

</xml_diff>